<commit_message>
-two sheets are changed. one deletion, one modification and one addition
</commit_message>
<xml_diff>
--- a/demo_file.xlsx
+++ b/demo_file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="plate 1" sheetId="5" r:id="rId1"/>
@@ -328,7 +328,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="67">
   <si>
     <t>A</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>BCA8</t>
+  </si>
+  <si>
+    <t>#this file has two changes: one deletion and one modification</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1464,9 +1467,6 @@
       <c r="H7">
         <v>0.34920001029968262</v>
       </c>
-      <c r="I7">
-        <v>0.42620000243186951</v>
-      </c>
       <c r="J7">
         <v>0.51169997453689575</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>0.10719999670982361</v>
       </c>
       <c r="F14">
-        <v>0.15279999375343323</v>
+        <v>0.1978</v>
       </c>
       <c r="G14">
         <v>0.11869999766349792</v>
@@ -2289,6 +2289,11 @@
         <v>58</v>
       </c>
       <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2300,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:M27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2559,9 +2564,6 @@
       <c r="B7">
         <v>7.3299996554851532E-2</v>
       </c>
-      <c r="C7">
-        <v>6.1000000685453415E-2</v>
-      </c>
       <c r="D7">
         <v>6.8099997937679291E-2</v>
       </c>
@@ -2812,7 +2814,7 @@
         <v>3.9500001817941666E-2</v>
       </c>
       <c r="E13">
-        <v>3.970000147819519E-2</v>
+        <v>0.99999000000000005</v>
       </c>
       <c r="F13">
         <v>0.11550000309944153</v>

</xml_diff>